<commit_message>
Added Row Names to .describe() output
</commit_message>
<xml_diff>
--- a/Data-Analysis/levelR1OnlyLiverMSDescription.xlsx
+++ b/Data-Analysis/levelR1OnlyLiverMSDescription.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>count</t>
   </si>
@@ -38,6 +38,78 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>Age at Diagnosis</t>
+  </si>
+  <si>
+    <t>MSIsensor Score</t>
+  </si>
+  <si>
+    <t>Metastasectomy</t>
+  </si>
+  <si>
+    <t>OS Months</t>
+  </si>
+  <si>
+    <t>Time to metastasis (months)</t>
+  </si>
+  <si>
+    <t>Time from Met Dx to Sequencing</t>
+  </si>
+  <si>
+    <t>Liver: First Site of Metastasis</t>
+  </si>
+  <si>
+    <t>Lymph Nodes: First Site of Metastasis</t>
+  </si>
+  <si>
+    <t>Lung: First Site of Metastasis</t>
+  </si>
+  <si>
+    <t>Pelvis: First Site of Metastasis</t>
+  </si>
+  <si>
+    <t>Brain: First Site of Metastasis</t>
+  </si>
+  <si>
+    <t>Bone: First Site of Metastasis</t>
+  </si>
+  <si>
+    <t>Peritoneum, omentum, abdomen: First Site of Metastasis</t>
+  </si>
+  <si>
+    <t>Gynecological: First Site of Metastasis</t>
+  </si>
+  <si>
+    <t>Other: First Site of Metastasis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of actionable alterations (OncoKb) </t>
+  </si>
+  <si>
+    <t>Samples for MSS Right/Left mCRC anslysis</t>
+  </si>
+  <si>
+    <t>Samples for MSS Right/Left analysis</t>
+  </si>
+  <si>
+    <t>Samples for MSS mCRC analysis</t>
+  </si>
+  <si>
+    <t>Hypermutated</t>
+  </si>
+  <si>
+    <t>Mutation Rate (mut/mb)</t>
+  </si>
+  <si>
+    <t>Fraction of Genome Altered</t>
+  </si>
+  <si>
+    <t>Ratio of Indel to Substitutions</t>
+  </si>
+  <si>
+    <t>Average Sample Alele Frequency</t>
   </si>
 </sst>
 </file>
@@ -395,103 +467,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
-        <v>321</v>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B2">
+        <v>321</v>
+      </c>
+      <c r="C2">
         <v>54.64485981308411</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>12.23308960599943</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>22</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>47</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>55</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>63</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
-        <v>321</v>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B3">
+        <v>321</v>
+      </c>
+      <c r="C3">
         <v>1.099906542056074</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>2.949439404995179</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
       <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>0.14</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.45</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1.16</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>32.04</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>321</v>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B4">
+        <v>321</v>
+      </c>
+      <c r="C4">
         <v>0.4548286604361371</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.4987328179256035</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
       <c r="E4">
         <v>0</v>
       </c>
@@ -499,51 +577,57 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
-        <v>321</v>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B5">
+        <v>321</v>
+      </c>
+      <c r="C5">
         <v>35.44283489096571</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>30.30569421124979</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.57</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>16.9</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>27.67</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>39.97</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>202.43</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
-        <v>321</v>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B6">
+        <v>321</v>
+      </c>
+      <c r="C6">
         <v>4.64953271034891</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>14.53156241508372</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
       <c r="E6">
         <v>0</v>
       </c>
@@ -554,50 +638,56 @@
         <v>0</v>
       </c>
       <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7">
-        <v>321</v>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B7">
+        <v>321</v>
+      </c>
+      <c r="C7">
         <v>22.54423675987849</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>28.97668331369515</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>-3.966666667</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>4.6</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>12</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>30.4</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>193.3333333</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8">
-        <v>321</v>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B8">
+        <v>321</v>
+      </c>
+      <c r="C8">
         <v>0.9937694704049844</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.07881027337873631</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -608,20 +698,23 @@
       <c r="H8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9">
-        <v>321</v>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B9">
+        <v>321</v>
+      </c>
+      <c r="C9">
         <v>0.1214953271028037</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>0.3272120978957619</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
       <c r="E9">
         <v>0</v>
       </c>
@@ -632,22 +725,25 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10">
-        <v>321</v>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B10">
+        <v>321</v>
+      </c>
+      <c r="C10">
         <v>0.1775700934579439</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>0.3827470798096362</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
       <c r="E10">
         <v>0</v>
       </c>
@@ -658,22 +754,25 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11">
-        <v>321</v>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B11">
+        <v>321</v>
+      </c>
+      <c r="C11">
         <v>0.02180685358255452</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>0.1462804671782308</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
       <c r="E11">
         <v>0</v>
       </c>
@@ -684,22 +783,25 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12">
-        <v>321</v>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B12">
+        <v>321</v>
+      </c>
+      <c r="C12">
         <v>0.009345794392523364</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>0.09637107023152787</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
       <c r="E12">
         <v>0</v>
       </c>
@@ -710,22 +812,25 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13">
-        <v>321</v>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B13">
+        <v>321</v>
+      </c>
+      <c r="C13">
         <v>0.01557632398753894</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>0.1240226589688138</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
       <c r="E13">
         <v>0</v>
       </c>
@@ -736,22 +841,25 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14">
-        <v>321</v>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B14">
+        <v>321</v>
+      </c>
+      <c r="C14">
         <v>0.1121495327102804</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>0.3160429995587524</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
       <c r="E14">
         <v>0</v>
       </c>
@@ -762,22 +870,25 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15">
-        <v>321</v>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B15">
+        <v>321</v>
+      </c>
+      <c r="C15">
         <v>0.0249221183800623</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>0.1561311853554529</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
       <c r="E15">
         <v>0</v>
       </c>
@@ -788,22 +899,25 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16">
-        <v>321</v>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B16">
+        <v>321</v>
+      </c>
+      <c r="C16">
         <v>0.02180685358255452</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>0.1462804671782309</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
       <c r="E16">
         <v>0</v>
       </c>
@@ -814,22 +928,25 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17">
-        <v>321</v>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B17">
+        <v>321</v>
+      </c>
+      <c r="C17">
         <v>0.4205607476635514</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>0.6476503181342831</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
       <c r="E17">
         <v>0</v>
       </c>
@@ -837,27 +954,30 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18">
-        <v>321</v>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B18">
+        <v>321</v>
+      </c>
+      <c r="C18">
         <v>0.940809968847352</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>0.2363484544064358</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -868,22 +988,25 @@
       <c r="H18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19">
-        <v>321</v>
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B19">
+        <v>321</v>
+      </c>
+      <c r="C19">
         <v>0.940809968847352</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>0.2363484544064358</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
       <c r="E19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -894,22 +1017,25 @@
       <c r="H19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20">
-        <v>321</v>
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B20">
+        <v>321</v>
+      </c>
+      <c r="C20">
         <v>0.9595015576323987</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>0.1974329019662527</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -920,20 +1046,23 @@
       <c r="H20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21">
-        <v>321</v>
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B21">
+        <v>321</v>
+      </c>
+      <c r="C21">
         <v>0.01869158878504673</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>0.1356448771988099</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
       <c r="E21">
         <v>0</v>
       </c>
@@ -944,110 +1073,125 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22">
-        <v>321</v>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B22">
+        <v>321</v>
+      </c>
+      <c r="C22">
         <v>6.992729278308408</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>15.38889817374895</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>0.833333333</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>4.347826087</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>5.072463768</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>6.52173913</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>207.5</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23">
-        <v>321</v>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B23">
+        <v>321</v>
+      </c>
+      <c r="C23">
         <v>0.1852783499937694</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>0.1546251534382728</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
       <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
         <v>0.052303586</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>0.157750376</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>0.272917337</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>0.758994206</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24">
-        <v>321</v>
+    <row r="24" spans="1:9">
+      <c r="A24" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B24">
+        <v>321</v>
+      </c>
+      <c r="C24">
         <v>0.2344874964299066</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>0.2462478661262735</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
         <v>0.166666667</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>0.333333333</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25">
-        <v>321</v>
+    <row r="25" spans="1:9">
+      <c r="A25" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B25">
+        <v>321</v>
+      </c>
+      <c r="C25">
         <v>0.464182640697819</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>0.1141909761538447</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>0.196648486</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>0.38358076</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>0.447825231</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>0.518538006</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>0.904696507</v>
       </c>
     </row>

</xml_diff>